<commit_message>
Various fixes related to GC data and sample collection
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/CIN/CH4_191_fisher/dataSheets/surgeData191.xlsx
+++ b/SuRGE_Sharepoint/data/CIN/CH4_191_fisher/dataSheets/surgeData191.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/CIN/CH4_191_fisher/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{C7F43E63-37B7-446B-B72C-C8C114541351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7300A961-DC0B-4357-BFD2-EB32DCFE269F}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{C7F43E63-37B7-446B-B72C-C8C114541351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38E07651-E375-47E9-AC95-DA45096DA4DD}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-105" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1332,10 +1332,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1373,7 +1377,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1479,7 +1483,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1621,7 +1625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1633,70 +1637,70 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L17" sqref="L17"/>
+      <selection pane="topRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="64" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="64" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="18" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>54</v>
       </c>
@@ -1778,7 +1782,7 @@
       <c r="BO1" s="30"/>
       <c r="BP1" s="30"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>162</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>0.59409722222222217</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>162</v>
       </c>
@@ -2219,7 +2223,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>162</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>162</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>162</v>
       </c>
@@ -2537,7 +2541,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>162</v>
       </c>
@@ -2641,7 +2645,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>162</v>
       </c>
@@ -2745,7 +2749,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>162</v>
       </c>
@@ -2849,7 +2853,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>162</v>
       </c>
@@ -2959,7 +2963,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>162</v>
       </c>
@@ -2993,10 +2997,10 @@
       <c r="L12" t="s">
         <v>203</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>204</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>205</v>
       </c>
       <c r="R12" t="s">
@@ -3072,7 +3076,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>162</v>
       </c>
@@ -3179,7 +3183,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>162</v>
       </c>
@@ -3283,7 +3287,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>162</v>
       </c>
@@ -3396,7 +3400,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>162</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>162</v>
       </c>
@@ -3630,14 +3634,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="116.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -3648,7 +3652,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3663,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3670,7 +3674,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -3681,7 +3685,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3692,7 +3696,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3703,7 +3707,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3714,7 +3718,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3725,7 +3729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3736,7 +3740,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3747,7 +3751,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3769,7 +3773,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3780,7 +3784,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3788,7 +3792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3799,7 +3803,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3807,7 +3811,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3818,7 +3822,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3826,7 +3830,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3837,7 +3841,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3848,7 +3852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3859,7 +3863,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3870,7 +3874,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3892,7 +3896,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3903,7 +3907,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3914,7 +3918,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3925,7 +3929,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3947,7 +3951,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -3958,7 +3962,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -3969,7 +3973,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -3977,7 +3981,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -3985,7 +3989,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -3993,7 +3997,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -4001,7 +4005,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -4009,7 +4013,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -4017,7 +4021,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>156</v>
       </c>
@@ -4025,7 +4029,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>141</v>
       </c>
@@ -4033,7 +4037,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>142</v>
       </c>
@@ -4041,7 +4045,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>143</v>
       </c>
@@ -4049,7 +4053,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>152</v>
       </c>
@@ -4057,7 +4061,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>144</v>
       </c>
@@ -4065,7 +4069,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -4076,7 +4080,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -4087,7 +4091,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -4098,7 +4102,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -4109,7 +4113,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -4120,7 +4124,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>153</v>
       </c>
@@ -4131,7 +4135,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -4142,7 +4146,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -4150,7 +4154,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -4158,7 +4162,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -4166,7 +4170,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -4174,7 +4178,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>154</v>
       </c>
@@ -4182,7 +4186,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -4190,7 +4194,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>145</v>
       </c>
@@ -4198,7 +4202,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>146</v>
       </c>
@@ -4206,7 +4210,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>147</v>
       </c>
@@ -4214,7 +4218,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>148</v>
       </c>
@@ -4222,7 +4226,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>155</v>
       </c>
@@ -4230,7 +4234,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -4238,7 +4242,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -4249,7 +4253,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -4260,7 +4264,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>51</v>
       </c>
@@ -4271,7 +4275,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>52</v>
       </c>
@@ -4282,7 +4286,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>53</v>
       </c>
@@ -4306,17 +4310,17 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="25"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="25"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>59</v>
       </c>
@@ -4332,7 +4336,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4366,7 +4370,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>162</v>
       </c>
@@ -4395,7 +4399,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>162</v>
       </c>
@@ -4424,7 +4428,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>162</v>
       </c>
@@ -4453,7 +4457,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>162</v>
       </c>
@@ -4482,7 +4486,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>162</v>
       </c>
@@ -4511,7 +4515,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>162</v>
       </c>
@@ -4558,14 +4562,14 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -4576,7 +4580,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4587,7 +4591,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4598,7 +4602,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>45</v>
       </c>
@@ -4609,7 +4613,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>46</v>
       </c>
@@ -4620,7 +4624,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>47</v>
       </c>
@@ -4631,7 +4635,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>48</v>
       </c>
@@ -4639,7 +4643,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>125</v>
       </c>
@@ -4650,7 +4654,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>126</v>
       </c>
@@ -4661,7 +4665,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>127</v>
       </c>
@@ -4672,7 +4676,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>160</v>
       </c>
@@ -4689,62 +4693,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d40b3e6283001fb57e5088f84fb23d5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aadbb8160917885bdc8cfb32badaafe9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5215,23 +5163,86 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{687AED28-C0C0-4CDB-9F92-0997580D8225}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="8b03727f-4454-4722-b3e6-018d8dcaf2fd"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5245,6 +5256,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{687AED28-C0C0-4CDB-9F92-0997580D8225}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>